<commit_message>
Atualizando a planilha de riscos
</commit_message>
<xml_diff>
--- a/entregaveis-grupo/documentacao/planilha-riscos.xlsx
+++ b/entregaveis-grupo/documentacao/planilha-riscos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Documents\FACULDADE\SPRINT2\WineTech\entregaveis-grupo\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C109CF2E-36AA-46C2-9CBF-B5133B806E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE7612D-DA22-4B25-8EE2-A332F9D0D77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -134,63 +134,42 @@
     <t>Mudança ambiental inesperada (ex: temperatura da adega varia rápido)</t>
   </si>
   <si>
-    <t>Grupo 11</t>
-  </si>
-  <si>
     <t>Vazamento de dados dos clientes</t>
   </si>
   <si>
     <t>Realizar auditorias de segurança periódicas.</t>
   </si>
   <si>
-    <t>Otavio</t>
-  </si>
-  <si>
     <t>Roubo ou dano físico dos sensores</t>
   </si>
   <si>
     <t>Orientar o cliente sobre segurança</t>
   </si>
   <si>
-    <t>Rafael</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aumento súbito no custo de componentes </t>
   </si>
   <si>
     <t>Manter estoque mínimo estratégico de componentes críticos.</t>
   </si>
   <si>
-    <t>Juan</t>
-  </si>
-  <si>
     <t>Lei seca no brasil, acarretando no fechamento de adegas</t>
   </si>
   <si>
     <t>Acompanhar legislações e políticas públicas do setor;</t>
   </si>
   <si>
-    <t>Marlon</t>
-  </si>
-  <si>
     <t xml:space="preserve">Atraso nas entregas das tasks </t>
   </si>
   <si>
     <t>Entregar a task para o membro que está mais livre</t>
   </si>
   <si>
-    <t>Yuri</t>
-  </si>
-  <si>
     <t>Um membro da equipe sair</t>
   </si>
   <si>
     <t>Reorganização das tasks da Sprint levando em conta a ausência do integrante</t>
   </si>
   <si>
-    <t>Leonardo</t>
-  </si>
-  <si>
     <t>Legenda</t>
   </si>
   <si>
@@ -198,13 +177,41 @@
   </si>
   <si>
     <t>Orientar o cliente sobre o controle de temperatura</t>
+  </si>
+  <si>
+    <t>PLANILHA DE RISCOS</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="36"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Aptos Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>WINE</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="36"/>
+        <color theme="1"/>
+        <rFont val="Aptos Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>TECH</t>
+    </r>
+  </si>
+  <si>
+    <t>Otavio Augusto / Leonardo Scavazza /  Juan Sanchez / Marlon Souza / Rafael Souza / Yuri Barcelos  GRUPO 11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,14 +235,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,8 +242,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <color rgb="FF7030A0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Aptos Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <color rgb="FF7030A0"/>
+      <name val="Aptos Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,24 +330,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="8" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -391,20 +438,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -412,7 +484,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -424,33 +496,54 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -795,7 +888,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="A22" sqref="A22:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -812,417 +905,423 @@
     <col min="13" max="13" width="69.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" s="13" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+    </row>
+    <row r="2" spans="1:13" ht="47.4" x14ac:dyDescent="0.9">
+      <c r="A2" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="G3" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2">
+        <v>6</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="8">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="2">
+        <v>3</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>6</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="8">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>3</v>
+      </c>
+      <c r="K6" s="2">
+        <v>6</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="8">
+        <v>4</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="G8" s="8">
+        <v>5</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G9" s="8">
+        <v>6</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2</v>
+      </c>
+      <c r="K9" s="2">
+        <v>4</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G10" s="8">
+        <v>7</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2">
+        <v>3</v>
+      </c>
+      <c r="K10" s="2">
+        <v>3</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G11" s="8">
+        <v>8</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G12" s="8">
+        <v>9</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2</v>
+      </c>
+      <c r="J12" s="2">
+        <v>3</v>
+      </c>
+      <c r="K12" s="2">
+        <v>6</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G13" s="8">
+        <v>10</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="I13" s="2">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G14" s="8">
+        <v>11</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="2">
+        <v>3</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
+      <c r="K14" s="2">
+        <v>6</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-      <c r="G9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G15" s="8">
+        <v>12</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="2">
         <v>1</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="J15" s="2">
         <v>3</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="3">
-        <v>2</v>
-      </c>
-      <c r="J10" s="3">
+      <c r="K15" s="2">
         <v>3</v>
       </c>
-      <c r="K10" s="3">
-        <v>6</v>
-      </c>
-      <c r="L10" s="3" t="s">
+      <c r="L15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="10">
-        <v>2</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="3">
-        <v>3</v>
-      </c>
-      <c r="J11" s="3">
-        <v>2</v>
-      </c>
-      <c r="K11" s="3">
-        <v>6</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="10">
-        <v>3</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="3">
-        <v>2</v>
-      </c>
-      <c r="J12" s="3">
-        <v>3</v>
-      </c>
-      <c r="K12" s="3">
-        <v>6</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="10">
-        <v>4</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="3">
-        <v>1</v>
-      </c>
-      <c r="J13" s="3">
-        <v>2</v>
-      </c>
-      <c r="K13" s="3">
-        <v>2</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="G14" s="10">
-        <v>5</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="3">
-        <v>1</v>
-      </c>
-      <c r="J14" s="3">
-        <v>1</v>
-      </c>
-      <c r="K14" s="3">
-        <v>1</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="G15" s="10">
-        <v>6</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I15" s="3">
-        <v>2</v>
-      </c>
-      <c r="J15" s="3">
-        <v>2</v>
-      </c>
-      <c r="K15" s="3">
-        <v>4</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="G16" s="10">
-        <v>7</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I16" s="3">
-        <v>1</v>
-      </c>
-      <c r="J16" s="3">
-        <v>3</v>
-      </c>
-      <c r="K16" s="3">
-        <v>3</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="G17" s="10">
-        <v>8</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" s="3">
-        <v>1</v>
-      </c>
-      <c r="J17" s="3">
-        <v>2</v>
-      </c>
-      <c r="K17" s="3">
-        <v>2</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="G18" s="10">
-        <v>9</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="3">
-        <v>2</v>
-      </c>
-      <c r="J18" s="3">
-        <v>3</v>
-      </c>
-      <c r="K18" s="3">
-        <v>6</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="G19" s="10">
-        <v>10</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I19" s="3">
-        <v>1</v>
-      </c>
-      <c r="J19" s="3">
-        <v>2</v>
-      </c>
-      <c r="K19" s="3">
-        <v>2</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M19" s="3" t="s">
+      <c r="M15" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="G20" s="10">
-        <v>11</v>
-      </c>
-      <c r="H20" s="5" t="s">
+    <row r="17" spans="1:8" ht="21" x14ac:dyDescent="0.3">
+      <c r="A17" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
         <v>44</v>
       </c>
-      <c r="I20" s="3">
-        <v>3</v>
-      </c>
-      <c r="J20" s="3">
-        <v>2</v>
-      </c>
-      <c r="K20" s="3">
-        <v>6</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="G21" s="10">
-        <v>12</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" s="3">
-        <v>1</v>
-      </c>
-      <c r="J21" s="3">
-        <v>3</v>
-      </c>
-      <c r="K21" s="3">
-        <v>3</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F25" t="s">
-        <v>51</v>
-      </c>
-      <c r="H25" s="14"/>
+      <c r="H25" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="A9:E9"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>